<commit_message>
Ajout croquis - guide organisateur
</commit_message>
<xml_diff>
--- a/excel/repas.xlsx
+++ b/excel/repas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47556BAC-8048-8D41-9E74-FE6B23A18202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7C4989-6763-6C4D-96BA-804A63102679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35420" yWindow="3200" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DEJEUNER" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
   <si>
     <t>code</t>
   </si>
@@ -153,12 +153,6 @@
     <t>100 % Pure Juice</t>
   </si>
   <si>
-    <t>Scrambled eggs, bacon, ham, sausage,roasted potatoes, pancake with syrup, cold cereal, oatmeal, banana, orange or apple, beverage  juice, milk, coffee)</t>
-  </si>
-  <si>
-    <t>Œufs brouillés, bacon, jambon, saucisse, pommes de terre rôties, crêpe avec sirop, céréales froides, gruau, banane, orange ou pomme, breuvage (jus,, lait, café)</t>
-  </si>
-  <si>
     <t>Soupe/potage, pain, spaghetti à la viande, mille-feuille graham, fruit, breuvage (jus ou lait, café)</t>
   </si>
   <si>
@@ -183,9 +177,6 @@
     <t>Soupe/potage, pain, lasagne, salade César, carré aux fraises, fruit, breuvage (jus ou lait, café)</t>
   </si>
   <si>
-    <t>Soup, bread, chicken salad panini, raw vegetables, cheese, indian orzo salad, cookies, fruit, beverage (juice or milk, coffee)</t>
-  </si>
-  <si>
     <t>**Boîte à lunch**&lt;br/&gt; Wrap à la viande froide, crudités, fromage, salade de macaroni, biscuits, orange, jus</t>
   </si>
   <si>
@@ -213,33 +204,6 @@
     <t>Soupe/potage, pain, pain viande sauce tomate, pomme de terre purée, légumes jardinière, gâteau au chocolat,  fruit, breuvage (jus ou lait, café)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Soupe/potage, pain, Assiette chinoise (riz, eggroll, légumes chinois, porc sauce sucrée, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>chicken ball)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, gâteau sucre à la crème, fruit, breuvage (jus ou lait, café)</t>
-    </r>
-  </si>
-  <si>
-    <t>Soup, bread, Chinese dish (rice, eggroll, chinese vegetables, pork in sweet sauce, chicken ball), sugar fudge cake, fruit, beverage (juice or milk, coffee)</t>
-  </si>
-  <si>
     <t>Soupe/potage, pain, suprême de poulet au gratin de poireaux, riz pilaf, jardinière de légumes, tarte au citron, fruit, breuvage (jus ou lait, café)</t>
   </si>
   <si>
@@ -261,7 +225,16 @@
     <t>Soup, bread, Italian spaghetti, graham mille-feuille, fruit, beverage (juice or milk, coffee)</t>
   </si>
   <si>
-    <t>Soupe/potage, pain, panini à la salade de poulet, crudités, fromage, salade d'orzo à l'indienne, biscuits, fruit, breuvage (jus ou lait, café)</t>
+    <t>Repas à Senneterre</t>
+  </si>
+  <si>
+    <t>Dinner at Senneterre</t>
+  </si>
+  <si>
+    <t>Œufs, bacon, jambon, saucisse, pommes de terre rôties, crêpe avec sirop, céréales froides, gruau, banane, orange ou pomme, breuvage (jus,, lait, café)</t>
+  </si>
+  <si>
+    <t>Eggs, bacon, ham, sausage,roasted potatoes, pancake with syrup, cold cereal, oatmeal, banana, orange or apple, beverage  juice, milk, coffee</t>
   </si>
 </sst>
 </file>
@@ -479,9 +452,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -519,7 +492,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -625,7 +598,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -767,7 +740,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -777,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -802,15 +775,15 @@
       </c>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="D2" s="5"/>
     </row>
@@ -878,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -908,10 +881,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D2" s="5"/>
     </row>
@@ -920,10 +893,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -932,10 +905,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -944,22 +917,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>50</v>
+      <c r="B6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="D6" s="5"/>
     </row>
@@ -968,10 +941,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D7" s="5"/>
     </row>
@@ -980,10 +953,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D8" s="6"/>
     </row>
@@ -1021,7 +994,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1050,10 +1023,10 @@
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D2" s="4"/>
     </row>
@@ -1062,10 +1035,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D3" s="5"/>
     </row>
@@ -1074,10 +1047,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -1086,10 +1059,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -1105,15 +1078,15 @@
       </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D7" s="5"/>
     </row>
@@ -1122,10 +1095,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D8" s="5"/>
     </row>
@@ -1134,10 +1107,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D9" s="6"/>
     </row>

</xml_diff>